<commit_message>
user cluster v1.0 (dataset: HIGH1000, HIGH20LOW100 done)
</commit_message>
<xml_diff>
--- a/Params.xlsx
+++ b/Params.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14800" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LIMIT 1000" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>条件</t>
     <rPh sb="0" eb="1">
@@ -72,31 +72,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">eps_percent = 0.60 min_samples = 50 </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">eps_percent = 0.70 min_samples = 40 </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>#Cls</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">eps_percent =  min_samples = </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">eps_percent =  min_samples =  </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>ORDER BY CNT_CASE (HIGH 20 + LOW 100)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>eps_percent = 0.85 min_samples = 15</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -121,19 +101,43 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">eps_percent =  min_samples = </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>match=1, mismatch=-1, gap=0</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>max_d = 0.3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>eps_percent = 0.40 min_samples = 10</t>
+    <t>max_d = 0.5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>eps = 30 min_samples = 10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>eps = 4  min_samples = 10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">eps = 40 min_samples = 10 </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>eps = 0.08 min_samples = 10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>eps = 0.90 min_samples = 10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">eps = 5 min_samples = 20 </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>eps = 0.01 min_samples = 10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>eps = 5 min_samples = 20</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -207,13 +211,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -232,39 +236,523 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>94400</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
+      <xdr:rowOff>119800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2050200</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>5500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="94400" y="1262800"/>
+          <a:ext cx="10058400" cy="5029200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>615156</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>178593</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>429418</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>108743</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26947812" y="13473906"/>
+          <a:ext cx="7315200" cy="5486400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2908281</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>90470</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>341294</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>20620</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11024375" y="13584220"/>
+          <a:ext cx="7315200" cy="5486400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>141250</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>22188</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>788950</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>150775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18972969" y="13515938"/>
+          <a:ext cx="7315200" cy="5486400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>615156</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>39688</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>429418</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>168275</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26947812" y="19486563"/>
+          <a:ext cx="7315200" cy="5486400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>189687</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>150000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>3950</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>80150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19021406" y="19596875"/>
+          <a:ext cx="7315200" cy="5486400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2840000</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>121407</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>273013</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>51557</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10956094" y="19568282"/>
+          <a:ext cx="7315200" cy="5486400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>595313</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26927969" y="1190625"/>
+          <a:ext cx="7315200" cy="5486400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2749531</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>149999</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>182544</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>80149</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10865625" y="1142187"/>
+          <a:ext cx="7315200" cy="5486400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>101562</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>141249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>749262</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>71399</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18933281" y="1133437"/>
+          <a:ext cx="7315200" cy="5486400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>290513</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>49212</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10973594" y="7262812"/>
+          <a:ext cx="7315200" cy="5486400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>626251</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7950200" y="1231900"/>
+      <xdr:rowOff>149999</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>440513</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>80149</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26958907" y="7095312"/>
           <a:ext cx="7315200" cy="5486400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -276,127 +764,39 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="203200" y="1219200"/>
-          <a:ext cx="7315200" cy="5486400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>121406</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="228600" y="6985000"/>
-          <a:ext cx="7315200" cy="5486400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7988300" y="7010400"/>
+      <xdr:rowOff>42032</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>769106</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>170619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18953125" y="7185782"/>
           <a:ext cx="7315200" cy="5486400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -413,20 +813,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>154586</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+      <xdr:rowOff>150422</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>7810</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>104383</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -445,7 +845,535 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6413500" y="1574800"/>
+          <a:off x="26369895" y="7111903"/>
+          <a:ext cx="7332113" cy="5410258"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>780835</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>121829</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>679235</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>83727</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10407749" y="7083310"/>
+          <a:ext cx="7345930" cy="5418195"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>434742</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>101172</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>293454</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>63071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18340174" y="7062653"/>
+          <a:ext cx="7337601" cy="5418196"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>106483</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>169983</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1235372"/>
+          <a:ext cx="10058714" cy="4955352"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>109753</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>141111</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>777052</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>171215</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26325062" y="1270000"/>
+          <a:ext cx="7315200" cy="5486400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>385186</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>87284</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>221497</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>117388</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18290618" y="1216173"/>
+          <a:ext cx="7315200" cy="5486400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>754691</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>49136</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>622361</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>79240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10381605" y="1178025"/>
+          <a:ext cx="7315200" cy="5486400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>955479</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>117279</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>822677</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>134683</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10607479" y="20030879"/>
+          <a:ext cx="7360198" cy="5910204"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>343479</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>140279</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>179790</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>185434</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26708679" y="20053879"/>
+          <a:ext cx="7380111" cy="5937955"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>87079</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>152931</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>761590</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>183034</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18908479" y="20066531"/>
+          <a:ext cx="7380111" cy="5922903"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26619200" y="13995400"/>
+          <a:ext cx="7315200" cy="5486400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>835800</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>73800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>658000</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>73800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10487800" y="13891400"/>
+          <a:ext cx="7315200" cy="5486400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>554000</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>122200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>325400</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>122200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18537200" y="13939800"/>
           <a:ext cx="7315200" cy="5486400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -723,8 +1651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView zoomScale="64" workbookViewId="0">
+      <selection activeCell="X67" sqref="X67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -746,13 +1674,13 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
@@ -766,16 +1694,16 @@
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="4">
-        <v>5</v>
+      <c r="F2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -783,14 +1711,14 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="4">
-        <v>3</v>
+      <c r="F3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="2">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -798,16 +1726,16 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="4">
-        <v>8</v>
+      <c r="F4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="2">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
@@ -815,24 +1743,24 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="4">
-        <v>4</v>
+      <c r="F5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="2">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="D1:F1"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="A2:A5"/>
-    <mergeCell ref="D1:F1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -845,8 +1773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -868,48 +1796,50 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="4"/>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="4">
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="2">
         <v>2</v>
       </c>
     </row>
@@ -918,28 +1848,32 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="4"/>
+      <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="4"/>
+      <c r="F5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
classify after clustering to extract features
</commit_message>
<xml_diff>
--- a/Params.xlsx
+++ b/Params.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="LIMIT 1000" sheetId="1" r:id="rId1"/>
@@ -212,10 +212,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1065,8 +1065,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="18290618" y="1216173"/>
-          <a:ext cx="7315200" cy="5486400"/>
+          <a:off x="18273016" y="1237473"/>
+          <a:ext cx="7276594" cy="5589349"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1651,8 +1651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="64" workbookViewId="0">
-      <selection activeCell="X67" sqref="X67"/>
+    <sheetView tabSelected="1" topLeftCell="J4" zoomScale="64" workbookViewId="0">
+      <selection activeCell="AK26" sqref="AK26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -1674,26 +1674,26 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
       <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -1707,10 +1707,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1722,10 +1722,10 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -1739,10 +1739,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
       <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1755,12 +1755,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A2:A5"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A2:A5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1773,8 +1773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView topLeftCell="H54" zoomScale="82" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -1796,26 +1796,26 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
       <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -1829,10 +1829,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1844,10 +1844,10 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -1861,10 +1861,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
       <c r="E5" s="2" t="s">
         <v>8</v>
       </c>

</xml_diff>